<commit_message>
Snapshot during implementation of thread-based worker class.  Basic thread structure set up, and output to console window is working.
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC315048-9F67-484E-AABC-AFDA0AB3AD62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F684E3-EE4F-FA41-BF24-F0F2ECC85A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35180" yWindow="5000" windowWidth="12220" windowHeight="11260" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="35540" yWindow="8000" windowWidth="12220" windowHeight="11260" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>✘</t>
-  </si>
-  <si>
-    <t>Fails</t>
   </si>
 </sst>
 </file>
@@ -449,7 +446,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B12" sqref="B12:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -488,69 +485,37 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -575,69 +540,33 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Converted path concatenations to use path.join instead of manual "/"
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Dropbox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F684E3-EE4F-FA41-BF24-F0F2ECC85A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B94B828-7CDE-9E4E-A3D6-3EFC2A42E115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35540" yWindow="8000" windowWidth="12220" windowHeight="11260" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="14460" yWindow="4280" windowWidth="14180" windowHeight="10580" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Median</t>
   </si>
   <si>
-    <t xml:space="preserve">MinMax </t>
-  </si>
-  <si>
     <t>Sigma</t>
   </si>
   <si>
@@ -69,13 +66,22 @@
   </si>
   <si>
     <t>✘</t>
+  </si>
+  <si>
+    <t>Two tests: complet and cancel</t>
+  </si>
+  <si>
+    <t>MinMax 1</t>
+  </si>
+  <si>
+    <t>MinMax 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -443,31 +449,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47930263-E802-DC48-8BED-3FA036517820}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="10.83203125" style="1"/>
+    <col min="2" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="4.1640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -475,54 +483,108 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -530,36 +592,75 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -567,6 +668,8 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished command line version
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Dropbox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B94B828-7CDE-9E4E-A3D6-3EFC2A42E115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971BEF33-DD8E-4646-BC67-AA073F0ADFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="4280" windowWidth="14180" windowHeight="10580" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="21660" yWindow="540" windowWidth="11580" windowHeight="10580" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -452,17 +452,17 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="4.1640625" style="1" customWidth="1"/>
     <col min="8" max="9" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,12 +470,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -492,7 +492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -516,7 +516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -537,7 +537,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -558,7 +558,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -579,12 +579,12 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -601,7 +601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -622,7 +622,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -643,32 +643,34 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated manual for clustering-based grouping
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971BEF33-DD8E-4646-BC67-AA073F0ADFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9473DDEF-5BE8-7941-B340-F21872457013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21660" yWindow="540" windowWidth="11580" windowHeight="10580" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="20440" yWindow="1220" windowWidth="12800" windowHeight="12880" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GUI" sheetId="1" r:id="rId1"/>
+    <sheet name="CmdLine" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="22">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -75,6 +76,30 @@
   </si>
   <si>
     <t>MinMax 2</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>By Size</t>
+  </si>
+  <si>
+    <t>By Exposure</t>
+  </si>
+  <si>
+    <t>By Temperature</t>
+  </si>
+  <si>
+    <t>Size and Exposure</t>
+  </si>
+  <si>
+    <t>Size and Temperature</t>
+  </si>
+  <si>
+    <t>Exposure and Temperature</t>
+  </si>
+  <si>
+    <t>All 3</t>
   </si>
 </sst>
 </file>
@@ -449,9 +474,615 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47930263-E802-DC48-8BED-3FA036517820}">
+  <dimension ref="A1:K59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="4.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FAB39DF-A927-524A-B817-296D45156A89}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated manual for clustering-based grouping, completed regression testing
</commit_message>
<xml_diff>
--- a/Testing Matrix.xlsx
+++ b/Testing Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/DropBox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Dropbox/dropbox/EWHO/Application Development/MasterDarkMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9473DDEF-5BE8-7941-B340-F21872457013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A9E793-9B22-224E-9563-848CF98E4379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20440" yWindow="1220" windowWidth="12800" windowHeight="12880" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12240" windowHeight="14780" xr2:uid="{CD4AAD33-191B-4341-AA11-41040B698EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="GUI" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="23">
   <si>
     <t>Single-file testing</t>
   </si>
@@ -100,13 +100,16 @@
   </si>
   <si>
     <t>All 3</t>
+  </si>
+  <si>
+    <t>Dispose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -474,20 +477,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47930263-E802-DC48-8BED-3FA036517820}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G56" activeCellId="1" sqref="F56 G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
     <col min="9" max="10" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,12 +498,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -520,68 +523,113 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H4" s="2"/>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -601,58 +649,107 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
@@ -672,58 +769,107 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
@@ -743,58 +889,107 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="B29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
@@ -814,19 +1009,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -838,7 +1043,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -848,7 +1053,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -860,12 +1065,12 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
@@ -885,11 +1090,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -897,19 +1104,23 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>2</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -919,7 +1130,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -927,16 +1138,20 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
@@ -956,11 +1171,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -968,7 +1185,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -980,7 +1197,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -990,7 +1207,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1002,12 +1219,12 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
@@ -1027,31 +1244,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -1061,7 +1286,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1072,6 +1297,14 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1086,14 +1319,14 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="4.1640625" style="1" customWidth="1"/>
     <col min="8" max="9" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1101,12 +1334,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1123,7 +1356,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1147,7 +1380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1168,7 +1401,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1422,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1210,12 +1443,12 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1232,7 +1465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1253,7 +1486,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1274,7 +1507,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1516,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>

</xml_diff>